<commit_message>
Adding fields to db table User
</commit_message>
<xml_diff>
--- a/tests/test_data_user.xlsx
+++ b/tests/test_data_user.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OneDrive - UNSW\University\Postgraduate\Year 3 Trimester 3\COMP9900\Project\BackEnd\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\CapstoneProject\comp9900-w17a-please-get-degrees-backend\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61FE47B3-20E8-4386-AFCB-CE637D6AF1BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD02959-5941-40E0-986E-C5D9297C176D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="21000" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -90,6 +81,45 @@
   </si>
   <si>
     <t>z5233368</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Jay</t>
+  </si>
+  <si>
+    <t>Meraachli</t>
+  </si>
+  <si>
+    <t>Brunette</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>Schroder</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Simon</t>
+  </si>
+  <si>
+    <t>Garrod</t>
+  </si>
+  <si>
+    <t>Kovid</t>
+  </si>
+  <si>
+    <t>Tim</t>
   </si>
 </sst>
 </file>
@@ -469,63 +499,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB9172-4BA3-48EB-851A-CC045B92290E}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C3">
+        <v>456</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C4">
+        <v>789</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C5">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C6">
+        <v>456</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DB updated and minor changes to signup and token
</commit_message>
<xml_diff>
--- a/tests/test_data_user.xlsx
+++ b/tests/test_data_user.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\CapstoneProject\comp9900-w17a-please-get-degrees-backend\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD02959-5941-40E0-986E-C5D9297C176D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FCDE71-2185-4077-AF2A-0D49F4C2A3A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Username</t>
-  </si>
-  <si>
-    <t>Email</t>
   </si>
   <si>
     <t>j.meraachli@student.unsw.edu.au</t>
@@ -86,12 +83,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
     <t>Jay</t>
   </si>
   <si>
@@ -120,6 +111,30 @@
   </si>
   <si>
     <t>Tim</t>
+  </si>
+  <si>
+    <t>jay</t>
+  </si>
+  <si>
+    <t>khan</t>
+  </si>
+  <si>
+    <t>kovid</t>
+  </si>
+  <si>
+    <t>simon</t>
+  </si>
+  <si>
+    <t>tim</t>
+  </si>
+  <si>
+    <t>Email_id</t>
+  </si>
+  <si>
+    <t>First_Name</t>
+  </si>
+  <si>
+    <t>Last_Name</t>
   </si>
 </sst>
 </file>
@@ -502,7 +517,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -516,101 +531,101 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>123</v>
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>456</v>
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>789</v>
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>123</v>
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>456</v>
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
configured database for watchlist and stocks. Wrote dummy data, extended dummy loader to load dummy data.
</commit_message>
<xml_diff>
--- a/tests/test_data_user.xlsx
+++ b/tests/test_data_user.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\CapstoneProject\comp9900-w17a-please-get-degrees-backend\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khan/PycharmProjects/comp9900-w17a-please-get-degrees-backend/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FCDE71-2185-4077-AF2A-0D49F4C2A3A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A10445-653E-2C4B-9592-810762081881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="2" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="users" sheetId="1" r:id="rId1"/>
+    <sheet name="watchlist" sheetId="2" r:id="rId2"/>
+    <sheet name="stock" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>Username</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>j.meraachli@student.unsw.edu.au</t>
   </si>
@@ -80,9 +79,6 @@
     <t>z5233368</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Jay</t>
   </si>
   <si>
@@ -128,20 +124,128 @@
     <t>tim</t>
   </si>
   <si>
-    <t>Email_id</t>
-  </si>
-  <si>
-    <t>First_Name</t>
-  </si>
-  <si>
-    <t>Last_Name</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>email_id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>other_name</t>
+  </si>
+  <si>
+    <t>date_joined</t>
+  </si>
+  <si>
+    <t>last_updated</t>
+  </si>
+  <si>
+    <t>validated</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>watchlist</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t>sim</t>
+  </si>
+  <si>
+    <t>sun</t>
+  </si>
+  <si>
+    <t>sibv</t>
+  </si>
+  <si>
+    <t>sdv</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>APPL</t>
+  </si>
+  <si>
+    <t>GOOG</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>AAAU</t>
+  </si>
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>stock_symbol</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>exchange</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>dvdsv</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>NYSE</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>fbfbdfb</t>
+  </si>
+  <si>
+    <t>saciuyt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +273,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,13 +301,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -514,118 +629,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB9172-4BA3-48EB-851A-CC045B92290E}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="J6" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -635,4 +808,287 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8D5324-5018-9640-9915-418B2F181888}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512DB6F3-F08F-9346-86EE-93C392BEFD26}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding portfolio portfolioprice transaction tables
</commit_message>
<xml_diff>
--- a/tests/test_data_user.xlsx
+++ b/tests/test_data_user.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\Desktop\comp9900-w17a-please-get-degrees-backend-dev\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\Desktop\test\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906B6349-8C1B-4B5E-8079-C3EC2C9EFE92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCE10AE-1DEC-472F-80FA-726E9B4583C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
     <sheet name="watchlist" sheetId="2" r:id="rId2"/>
     <sheet name="stock" sheetId="3" r:id="rId3"/>
+    <sheet name="portfolio" sheetId="4" r:id="rId4"/>
+    <sheet name="portfolioprice" sheetId="5" r:id="rId5"/>
+    <sheet name="transaction" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="76">
   <si>
     <t>j.meraachli@student.unsw.edu.au</t>
   </si>
@@ -187,6 +190,18 @@
     <t>USA</t>
   </si>
   <si>
+    <t>portfolio_id</t>
+  </si>
+  <si>
+    <t>portfolio_name</t>
+  </si>
+  <si>
+    <t>close_balance</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
     <t>DELL</t>
   </si>
   <si>
@@ -209,6 +224,60 @@
   </si>
   <si>
     <t>KPMG Ltd</t>
+  </si>
+  <si>
+    <t>Khans Portfolio One</t>
+  </si>
+  <si>
+    <t>Jays Portfolio One</t>
+  </si>
+  <si>
+    <t>Jays Portfolio Two</t>
+  </si>
+  <si>
+    <t>Tims Portfolio</t>
+  </si>
+  <si>
+    <t>Kovids Portfolio</t>
+  </si>
+  <si>
+    <t>Simons Portfolio</t>
+  </si>
+  <si>
+    <t>Khans Portfolio Two</t>
+  </si>
+  <si>
+    <t>transaction</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>trade_type</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>fee</t>
+  </si>
+  <si>
+    <t>portfolio</t>
+  </si>
+  <si>
+    <t>portfolio_price</t>
+  </si>
+  <si>
+    <t>settled</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>sell</t>
+  </si>
+  <si>
+    <t>Tims Portfolio Two</t>
   </si>
 </sst>
 </file>
@@ -271,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -284,6 +353,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -599,19 +670,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB9172-4BA3-48EB-851A-CC045B92290E}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -639,8 +713,14 @@
       <c r="I1" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -655,11 +735,14 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
       <c r="H2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -674,11 +757,14 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
       <c r="H3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -693,11 +779,14 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
       <c r="H4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -712,11 +801,14 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
       <c r="H5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -731,13 +823,16 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
       <c r="H6" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{3AED0E9E-D16B-4A5B-964D-D80C0CE0C4CB}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{73480234-B25F-499D-AC8A-F116F644BDCD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -749,7 +844,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B17"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -784,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -792,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -800,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -828,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -838,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -848,7 +943,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -875,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -884,7 +979,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -892,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -900,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -912,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512DB6F3-F08F-9346-86EE-93C392BEFD26}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -980,10 +1075,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>42</v>
@@ -1000,10 +1095,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>42</v>
@@ -1020,10 +1115,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
         <v>42</v>
@@ -1040,10 +1135,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
@@ -1061,4 +1156,968 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51161AFF-7779-4BC8-A52D-606E943847CF}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9448928-3915-4856-835A-5C489B392B12}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>10000</v>
+      </c>
+      <c r="D2" s="7">
+        <v>44119.108414351853</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="7">
+        <v>44119.150081018517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="7">
+        <v>44119.191747685189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+      <c r="D5" s="7">
+        <v>44119.233414351853</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>10000</v>
+      </c>
+      <c r="D6" s="7">
+        <v>44119.275081018517</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10000</v>
+      </c>
+      <c r="D7" s="7">
+        <v>44119.316747685189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>10000</v>
+      </c>
+      <c r="D8" s="7">
+        <v>44119.358414351853</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="7">
+        <v>44120.441747685189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839B1F08-9FB4-4205-9D29-58AB9BDB11FE}">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="7">
+        <v>44119.108414351853</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="7">
+        <v>44119.108414351853</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="6">
+        <v>44119.108419884258</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="6">
+        <v>44119.108419884258</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="6">
+        <v>44119.108419884258</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="7">
+        <v>44119.108414351853</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="7">
+        <v>44119.233414351853</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="7">
+        <v>44119.275081018517</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G18">
+        <v>90</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G19">
+        <v>1200</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G20">
+        <v>90</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G21">
+        <v>1200</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>60</v>
+      </c>
+      <c r="E22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G22">
+        <v>190</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>60</v>
+      </c>
+      <c r="E24" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G24">
+        <v>190</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25">
+        <v>60</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G25">
+        <v>100</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding portfolio, portfolioprice and transactions
</commit_message>
<xml_diff>
--- a/tests/test_data_user.xlsx
+++ b/tests/test_data_user.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\Desktop\comp9900-w17a-please-get-degrees-backend-dev\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kovid\Desktop\d\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906B6349-8C1B-4B5E-8079-C3EC2C9EFE92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69F487F-72C8-446B-B60A-0C4C31BF5761}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{1A28855D-1372-4992-8C97-28705A0C69E1}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
     <sheet name="watchlist" sheetId="2" r:id="rId2"/>
     <sheet name="stock" sheetId="3" r:id="rId3"/>
+    <sheet name="portfolio" sheetId="4" r:id="rId4"/>
+    <sheet name="portfolioprice" sheetId="5" r:id="rId5"/>
+    <sheet name="transaction" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="69">
   <si>
     <t>j.meraachli@student.unsw.edu.au</t>
   </si>
@@ -94,21 +97,6 @@
     <t>Tim</t>
   </si>
   <si>
-    <t>jay</t>
-  </si>
-  <si>
-    <t>khan</t>
-  </si>
-  <si>
-    <t>kovid</t>
-  </si>
-  <si>
-    <t>simon</t>
-  </si>
-  <si>
-    <t>tim</t>
-  </si>
-  <si>
     <t>email_id</t>
   </si>
   <si>
@@ -187,6 +175,18 @@
     <t>USA</t>
   </si>
   <si>
+    <t>portfolio_id</t>
+  </si>
+  <si>
+    <t>portfolio_name</t>
+  </si>
+  <si>
+    <t>close_balance</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
     <t>DELL</t>
   </si>
   <si>
@@ -209,13 +209,61 @@
   </si>
   <si>
     <t>KPMG Ltd</t>
+  </si>
+  <si>
+    <t>transaction</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>trade_type</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>fee</t>
+  </si>
+  <si>
+    <t>portfolio</t>
+  </si>
+  <si>
+    <t>portfolio_price</t>
+  </si>
+  <si>
+    <t>settled</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>sell</t>
+  </si>
+  <si>
+    <t>pass1234</t>
+  </si>
+  <si>
+    <t>Jay's Portfolio</t>
+  </si>
+  <si>
+    <t>Khan's Portfolio</t>
+  </si>
+  <si>
+    <t>Kovid's Portfolio</t>
+  </si>
+  <si>
+    <t>Simon's Portfolio</t>
+  </si>
+  <si>
+    <t>Tim's Portfolio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +297,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -271,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -284,6 +338,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -599,53 +655,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36BB9172-4BA3-48EB-851A-CC045B92290E}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -655,16 +720,19 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
       <c r="H2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -674,16 +742,19 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
       <c r="H3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -693,16 +764,19 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
       <c r="H4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -712,16 +786,19 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
       <c r="H5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -731,13 +808,17 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{3AED0E9E-D16B-4A5B-964D-D80C0CE0C4CB}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{73480234-B25F-499D-AC8A-F116F644BDCD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -749,17 +830,17 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B17"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -767,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -775,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -784,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -792,7 +873,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -800,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -808,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -818,7 +899,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -828,7 +909,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -838,7 +919,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -848,7 +929,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -857,7 +938,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -866,7 +947,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -875,7 +956,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -884,7 +965,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -892,7 +973,7 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -900,7 +981,7 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -912,153 +993,910 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512DB6F3-F08F-9346-86EE-93C392BEFD26}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51161AFF-7779-4BC8-A52D-606E943847CF}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9448928-3915-4856-835A-5C489B392B12}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>10000</v>
+      </c>
+      <c r="D2" s="7">
+        <v>44119.108414351853</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10000</v>
+      </c>
+      <c r="D3" s="7">
+        <v>44119.150081018517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10000</v>
+      </c>
+      <c r="D4" s="7">
+        <v>44119.191747685189</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+      <c r="D5" s="7">
+        <v>44119.233414351853</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>10000</v>
+      </c>
+      <c r="D6" s="7">
+        <v>44119.275081018517</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839B1F08-9FB4-4205-9D29-58AB9BDB11FE}">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A16:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="7">
+        <v>44119.108414351853</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="7">
+        <v>44119.108414351853</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="6">
+        <v>44119.108419884258</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="6">
+        <v>44119.108419884258</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="6">
+        <v>44119.108419884258</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="7">
+        <v>44119.108414351853</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="7">
+        <v>44119.233414351853</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="7">
+        <v>44119.275081018517</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="7">
+        <v>44119.441747685189</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G18">
+        <v>90</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G19">
+        <v>1200</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G20">
+        <v>90</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="7">
+        <v>44119.483414351853</v>
+      </c>
+      <c r="G21">
+        <v>1200</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="F25" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>